<commit_message>
Generating arbitary circle in 3D space and tracking it
</commit_message>
<xml_diff>
--- a/IndyRP2_configure.xlsx
+++ b/IndyRP2_configure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MECH639\mech639_pybullet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C639BD-00A7-4FA8-8B74-AD8E61CDCB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43CB6FD-30C3-4835-9F8D-62ACF46ABA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0A9398FC-6F38-4698-9702-314029B441A4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A9398FC-6F38-4698-9702-314029B441A4}"/>
   </bookViews>
   <sheets>
     <sheet name="PositionOrientation" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -158,6 +158,10 @@
   </si>
   <si>
     <t>max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -864,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01C0089-5F20-42AB-9269-204A46CF6CD9}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -908,6 +912,12 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3">
+        <v>7.7499999999999999E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -923,11 +933,11 @@
         <v>1.2669999999999999</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E3:E8" si="0">D4-D5</f>
+        <f t="shared" ref="E4:E8" si="0">D4-D5</f>
         <v>0.16799999999999993</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F3:F8" si="1">C4-C5</f>
+        <f t="shared" ref="F4:F8" si="1">C4-C5</f>
         <v>-6.9000000000000006E-2</v>
       </c>
       <c r="G4">
@@ -940,15 +950,15 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <f>C4*I4+D4*H4</f>
+        <f t="shared" ref="J4:J8" si="2">C4*I4-D4*H4</f>
         <v>-0.18640000000000001</v>
       </c>
       <c r="K4">
-        <f>D4*G4+B4*I4</f>
+        <f>D4*G4-B4*I4</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>B4*H4+C4*G4</f>
+        <f>B4*H4-C4*G4</f>
         <v>0</v>
       </c>
       <c r="N4" t="s">
@@ -990,15 +1000,15 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J10" si="2">C5*I5+D5*H5</f>
-        <v>-1.099</v>
+        <f t="shared" ref="J5:J10" si="3">C5*I5-D5*H5</f>
+        <v>1.099</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K10" si="3">D5*G5+B5*I5</f>
+        <f t="shared" ref="K5:K10" si="4">D5*G5-B5*I5</f>
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L10" si="4">B5*H5+C5*G5</f>
+        <f t="shared" ref="L5:L10" si="5">B5*H5-C5*G5</f>
         <v>0</v>
       </c>
       <c r="N5" t="s">
@@ -1040,15 +1050,15 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.3999999999999998E-3</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N6" t="s">
@@ -1090,15 +1100,15 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>-0.749</v>
+        <f t="shared" si="3"/>
+        <v>0.749</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N7" t="s">
@@ -1140,15 +1150,15 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.19370000000000001</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N8" t="s">
@@ -1190,15 +1200,15 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
-        <v>-0.29949999999999999</v>
+        <f t="shared" si="3"/>
+        <v>0.29949999999999999</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N9" t="s">
@@ -1222,6 +1232,13 @@
       <c r="D10">
         <v>7.7499999999999999E-2</v>
       </c>
+      <c r="E10">
+        <f>D10</f>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="G10">
         <v>0</v>
       </c>
@@ -1232,15 +1249,15 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N10" t="s">
@@ -1315,12 +1332,15 @@
         <v>6</v>
       </c>
       <c r="B16">
+        <f t="shared" ref="B16:B21" si="6">J4</f>
         <v>-0.18640000000000001</v>
       </c>
       <c r="C16">
+        <f t="shared" ref="C16:C21" si="7">K4</f>
         <v>0</v>
       </c>
       <c r="D16">
+        <f t="shared" ref="D16:D21" si="8">L4</f>
         <v>0</v>
       </c>
       <c r="E16">
@@ -1345,12 +1365,15 @@
         <v>5</v>
       </c>
       <c r="B17">
-        <v>-1.099</v>
+        <f t="shared" si="6"/>
+        <v>1.099</v>
       </c>
       <c r="C17">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D17">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E17">
@@ -1368,12 +1391,15 @@
         <v>4</v>
       </c>
       <c r="B18">
+        <f t="shared" si="6"/>
         <v>-3.3999999999999998E-3</v>
       </c>
       <c r="C18">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D18">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E18">
@@ -1391,12 +1417,15 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>-0.749</v>
+        <f t="shared" si="6"/>
+        <v>0.749</v>
       </c>
       <c r="C19">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D19">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E19">
@@ -1414,12 +1443,15 @@
         <v>2</v>
       </c>
       <c r="B20">
+        <f t="shared" si="6"/>
         <v>-0.19370000000000001</v>
       </c>
       <c r="C20">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D20">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E20">
@@ -1437,12 +1469,15 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>-0.29949999999999999</v>
+        <f t="shared" si="6"/>
+        <v>0.29949999999999999</v>
       </c>
       <c r="C21">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D21">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E21">
@@ -1460,12 +1495,15 @@
         <v>0</v>
       </c>
       <c r="B22">
+        <f>J10</f>
         <v>0</v>
       </c>
       <c r="C22">
+        <f t="shared" ref="C22:D22" si="9">K10</f>
         <v>0</v>
       </c>
       <c r="D22">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E22">
@@ -1528,11 +1566,11 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E26:E31" si="5">D27-D28</f>
+        <f t="shared" ref="E27:E31" si="10">D27-D28</f>
         <v>0.16799999999999993</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F26:F31" si="6">C27-C28</f>
+        <f t="shared" ref="F27:F31" si="11">C27-C28</f>
         <v>-6.9000000000000006E-2</v>
       </c>
       <c r="G27">
@@ -1545,15 +1583,15 @@
         <v>1</v>
       </c>
       <c r="J27">
-        <f>C27*I27+D27*H27</f>
+        <f t="shared" ref="J27:J32" si="12">C27*I27-D27*H27</f>
         <v>0</v>
       </c>
       <c r="K27">
-        <f>D27*G27+B27*I27</f>
+        <f>D27*G27-B27*I27</f>
         <v>0</v>
       </c>
       <c r="L27">
-        <f>B27*H27+C27*G27</f>
+        <f>B27*H27-C27*G27</f>
         <v>0</v>
       </c>
     </row>
@@ -1573,11 +1611,11 @@
         <v>-0.16799999999999993</v>
       </c>
       <c r="E28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.2999999999999963E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-0.11399999999999999</v>
       </c>
       <c r="G28">
@@ -1590,15 +1628,15 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28:J33" si="7">C28*I28+D28*H28</f>
-        <v>0.16799999999999993</v>
+        <f t="shared" ref="J28:J33" si="13">C28*I28-D28*H28</f>
+        <v>-0.16799999999999993</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:K33" si="8">D28*G28+B28*I28</f>
+        <f t="shared" ref="K28:K33" si="14">D28*G28-B28*I28</f>
         <v>0</v>
       </c>
       <c r="L28">
-        <f t="shared" ref="L28:L33" si="9">B28*H28+C28*G28</f>
+        <f t="shared" ref="L28:L33" si="15">B28*H28-C28*G28</f>
         <v>0</v>
       </c>
     </row>
@@ -1618,11 +1656,11 @@
         <v>-0.25099999999999989</v>
       </c>
       <c r="E29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.26700000000000002</v>
       </c>
       <c r="F29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G29">
@@ -1635,15 +1673,15 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.183</v>
       </c>
       <c r="K29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -1663,11 +1701,11 @@
         <v>-0.5179999999999999</v>
       </c>
       <c r="E30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>6.5500000000000003E-2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.11530000000000001</v>
       </c>
       <c r="G30">
@@ -1680,15 +1718,15 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <f t="shared" si="7"/>
-        <v>0.5179999999999999</v>
+        <f t="shared" si="13"/>
+        <v>-0.5179999999999999</v>
       </c>
       <c r="K30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -1708,11 +1746,11 @@
         <v>-0.58349999999999991</v>
       </c>
       <c r="E31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.38400000000000001</v>
       </c>
       <c r="F31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-8.4700000000000011E-2</v>
       </c>
       <c r="G31">
@@ -1725,15 +1763,15 @@
         <v>1</v>
       </c>
       <c r="J31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>-7.3000000000000148E-3</v>
       </c>
       <c r="K31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -1770,15 +1808,15 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <f t="shared" si="7"/>
-        <v>0.96749999999999992</v>
+        <f t="shared" si="13"/>
+        <v>-0.96749999999999992</v>
       </c>
       <c r="K32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -1807,15 +1845,15 @@
         <v>1</v>
       </c>
       <c r="J33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.18640000000000001</v>
       </c>
       <c r="K33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -1848,12 +1886,15 @@
         <v>6</v>
       </c>
       <c r="B39">
+        <f t="shared" ref="B39:B44" si="16">J27</f>
         <v>0</v>
       </c>
       <c r="C39">
+        <f t="shared" ref="C39:C44" si="17">K27</f>
         <v>0</v>
       </c>
       <c r="D39">
+        <f t="shared" ref="D39:D44" si="18">L27</f>
         <v>0</v>
       </c>
       <c r="E39">
@@ -1871,12 +1912,15 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>0.16799999999999993</v>
+        <f t="shared" si="16"/>
+        <v>-0.16799999999999993</v>
       </c>
       <c r="C40">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D40">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E40">
@@ -1894,12 +1938,15 @@
         <v>4</v>
       </c>
       <c r="B41">
+        <f t="shared" si="16"/>
         <v>0.183</v>
       </c>
       <c r="C41">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D41">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E41">
@@ -1917,12 +1964,15 @@
         <v>3</v>
       </c>
       <c r="B42">
-        <v>0.5179999999999999</v>
+        <f t="shared" si="16"/>
+        <v>-0.5179999999999999</v>
       </c>
       <c r="C42">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D42">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E42">
@@ -1940,12 +1990,15 @@
         <v>2</v>
       </c>
       <c r="B43">
+        <f t="shared" si="16"/>
         <v>-7.3000000000000148E-3</v>
       </c>
       <c r="C43">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D43">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E43">
@@ -1963,12 +2016,15 @@
         <v>1</v>
       </c>
       <c r="B44">
-        <v>0.96749999999999992</v>
+        <f t="shared" si="16"/>
+        <v>-0.96749999999999992</v>
       </c>
       <c r="C44">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D44">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E44">
@@ -1986,12 +2042,15 @@
         <v>0</v>
       </c>
       <c r="B45">
+        <f>J33</f>
         <v>0.18640000000000001</v>
       </c>
       <c r="C45">
+        <f t="shared" ref="C45:D45" si="19">K33</f>
         <v>0</v>
       </c>
       <c r="D45">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E45">
@@ -2015,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEECD24-8550-41D2-90F4-DA53AC029D50}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>